<commit_message>
Added code to perform both GET and POST
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\go_code\src\github.com\dminGod\Tsetse-Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek\Tsetse-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16812" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="233">
   <si>
     <t>/v1/product/productSpecification/productMaster.json?filter=(&amp;(matCode_key15=02))</t>
   </si>
@@ -711,6 +711,18 @@
   </si>
   <si>
     <t>/v1/sales/salesStatistic/printHistoryDetail.json?filter=(|(transactionId=03)(transactionType=History))</t>
+  </si>
+  <si>
+    <t>Test_Call_Abhishek_POST</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/SLA1/Sid</t>
+  </si>
+  <si>
+    <t>test1.json</t>
   </si>
 </sst>
 </file>
@@ -1028,19 +1040,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="124.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1051,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1073,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1084,7 +1097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1106,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1117,7 +1130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1139,7 +1152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1161,7 +1174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1183,7 +1196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1194,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1205,7 +1218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1216,7 +1229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1227,7 +1240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1238,7 +1251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1249,7 +1262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1260,7 +1273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1271,7 +1284,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1282,7 +1295,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1293,7 +1306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1304,7 +1317,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1315,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1326,7 +1339,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1337,7 +1350,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1348,7 +1361,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1359,7 +1372,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1370,7 +1383,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1381,7 +1394,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1392,7 +1405,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1414,7 +1427,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1425,7 +1438,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1436,7 +1449,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1447,7 +1460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1458,7 +1471,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1469,7 +1482,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1480,7 +1493,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1491,7 +1504,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1513,7 +1526,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -1535,7 +1548,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -1546,7 +1559,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -1557,7 +1570,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -1568,7 +1581,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -1579,7 +1592,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -1590,7 +1603,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -1601,7 +1614,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -1612,7 +1625,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -1623,7 +1636,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -1634,7 +1647,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -1645,7 +1658,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -1656,7 +1669,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -1667,7 +1680,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -1678,7 +1691,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -1689,7 +1702,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -1700,7 +1713,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -1711,7 +1724,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -1722,7 +1735,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -1733,7 +1746,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -1744,7 +1757,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -1755,7 +1768,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -1766,7 +1779,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -1777,7 +1790,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -1788,7 +1801,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -1799,7 +1812,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -1810,7 +1823,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>137</v>
       </c>
@@ -1821,7 +1834,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -1832,7 +1845,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -1843,7 +1856,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -1854,7 +1867,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -1865,7 +1878,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -1876,7 +1889,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>149</v>
       </c>
@@ -1887,7 +1900,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>151</v>
       </c>
@@ -1898,7 +1911,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -1909,7 +1922,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>155</v>
       </c>
@@ -1920,7 +1933,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>157</v>
       </c>
@@ -1931,7 +1944,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -1942,7 +1955,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>161</v>
       </c>
@@ -1953,7 +1966,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>163</v>
       </c>
@@ -1964,7 +1977,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -1975,7 +1988,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>167</v>
       </c>
@@ -1986,7 +1999,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -1997,7 +2010,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -2008,7 +2021,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>173</v>
       </c>
@@ -2019,7 +2032,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -2030,7 +2043,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -2041,7 +2054,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>179</v>
       </c>
@@ -2052,7 +2065,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>180</v>
       </c>
@@ -2063,7 +2076,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>182</v>
       </c>
@@ -2074,7 +2087,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>116</v>
       </c>
@@ -2085,7 +2098,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>118</v>
       </c>
@@ -2096,7 +2109,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>120</v>
       </c>
@@ -2107,7 +2120,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>122</v>
       </c>
@@ -2118,7 +2131,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -2129,7 +2142,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>125</v>
       </c>
@@ -2140,7 +2153,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>127</v>
       </c>
@@ -2151,7 +2164,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>129</v>
       </c>
@@ -2162,7 +2175,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>131</v>
       </c>
@@ -2173,7 +2186,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>133</v>
       </c>
@@ -2184,7 +2197,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>135</v>
       </c>
@@ -2195,7 +2208,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>137</v>
       </c>
@@ -2206,7 +2219,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>139</v>
       </c>
@@ -2217,7 +2230,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>141</v>
       </c>
@@ -2228,7 +2241,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>143</v>
       </c>
@@ -2239,7 +2252,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>145</v>
       </c>
@@ -2250,7 +2263,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>147</v>
       </c>
@@ -2261,7 +2274,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>149</v>
       </c>
@@ -2272,7 +2285,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>151</v>
       </c>
@@ -2283,7 +2296,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>153</v>
       </c>
@@ -2294,7 +2307,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -2305,7 +2318,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>157</v>
       </c>
@@ -2316,7 +2329,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>159</v>
       </c>
@@ -2327,7 +2340,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>161</v>
       </c>
@@ -2338,7 +2351,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>163</v>
       </c>
@@ -2349,7 +2362,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>165</v>
       </c>
@@ -2360,7 +2373,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>167</v>
       </c>
@@ -2371,7 +2384,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>169</v>
       </c>
@@ -2382,7 +2395,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>171</v>
       </c>
@@ -2393,7 +2406,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>173</v>
       </c>
@@ -2404,7 +2417,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>175</v>
       </c>
@@ -2415,7 +2428,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>177</v>
       </c>
@@ -2426,7 +2439,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>179</v>
       </c>
@@ -2437,7 +2450,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>180</v>
       </c>
@@ -2448,7 +2461,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>182</v>
       </c>
@@ -2459,7 +2472,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>28</v>
       </c>
@@ -2470,7 +2483,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>30</v>
       </c>
@@ -2481,7 +2494,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>32</v>
       </c>
@@ -2492,7 +2505,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2516,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>36</v>
       </c>
@@ -2514,7 +2527,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>38</v>
       </c>
@@ -2525,7 +2538,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>40</v>
       </c>
@@ -2536,7 +2549,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -2547,7 +2560,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>44</v>
       </c>
@@ -2558,7 +2571,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>46</v>
       </c>
@@ -2569,7 +2582,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>48</v>
       </c>
@@ -2578,6 +2591,20 @@
       </c>
       <c r="C140" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>229</v>
+      </c>
+      <c r="B141" t="s">
+        <v>230</v>
+      </c>
+      <c r="C141" t="s">
+        <v>231</v>
+      </c>
+      <c r="D141" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>